<commit_message>
Auto-committed on 2023/02/24 週五 18:28:06.70
</commit_message>
<xml_diff>
--- a/Program/Other/L9707_底稿_新增逾放案件明細.xlsx
+++ b/Program/Other/L9707_底稿_新增逾放案件明細.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\itxWrite\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6816E00-289C-4C5C-BB7D-191690BCDE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="D9701212" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$2:$N$116</definedName>
-    <definedName name="_xlnm.Database">工作表1!$A$2:$N$116</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">D9701212!$A$2:$N$116</definedName>
+    <definedName name="_xlnm.Database">D9701212!$A$2:$N$116</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -124,7 +125,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0.00_ "/>
@@ -762,7 +763,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -771,9 +772,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -931,6 +929,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -966,6 +981,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1141,28 +1173,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="9.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" style="1" customWidth="1"/>
-    <col min="5" max="7" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.6640625" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13" max="14" width="4.77734375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" customWidth="1"/>
+    <col min="1" max="2" width="9.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6328125" style="1" customWidth="1"/>
+    <col min="5" max="7" width="12.6328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6328125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.6328125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6328125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="4.81640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1206,55 +1238,55 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O3" s="10"/>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="O3" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:N116"/>
+  <autoFilter ref="A2:N116" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>